<commit_message>
Results from June 28, 2020 11:39 pm CT run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-06-28.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-06-28.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -358,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,25 +430,1176 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C2" t="n">
+        <v>31752</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1310</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1311</v>
+      </c>
+      <c r="F2" t="n">
+        <v>40</v>
+      </c>
+      <c r="G2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C3" t="n">
+        <v>27743</v>
+      </c>
+      <c r="D3" t="n">
+        <v>777</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4866</v>
+      </c>
+      <c r="F3" t="n">
+        <v>183</v>
+      </c>
+      <c r="G3" t="n">
+        <v>19.6</v>
+      </c>
+      <c r="H3" t="n">
+        <v>23.92</v>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Wisconsin -- Milwaukee</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C4" t="n">
+        <v>11064</v>
+      </c>
+      <c r="D4" t="n">
+        <v>352</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3092</v>
+      </c>
+      <c r="F4" t="n">
+        <v>141</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30.26</v>
+      </c>
+      <c r="H4" t="n">
+        <v>40.06</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rhode Island</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44004</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15948</v>
+      </c>
+      <c r="D5" t="n">
+        <v>903</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1535</v>
+      </c>
+      <c r="F5" t="n">
+        <v>46</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12.31</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.18</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Maine</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3191</v>
+      </c>
+      <c r="D6" t="n">
+        <v>104</v>
+      </c>
+      <c r="E6" t="n">
+        <v>761</v>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>27.1</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
           <t>Maryland</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>An error occurred. ... WebDriverException('Can not connect to the Service chromedriver')</t>
+      <c r="B7" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C7" t="n">
+        <v>66777</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3042</v>
+      </c>
+      <c r="E7" t="n">
+        <v>19122</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1238</v>
+      </c>
+      <c r="G7" t="n">
+        <v>28.64</v>
+      </c>
+      <c r="H7" t="n">
+        <v>40.7</v>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C8" t="n">
+        <v>34964</v>
+      </c>
+      <c r="D8" t="n">
+        <v>898</v>
+      </c>
+      <c r="E8" t="n">
+        <v>13430</v>
+      </c>
+      <c r="F8" t="n">
+        <v>413</v>
+      </c>
+      <c r="G8" t="n">
+        <v>47.85</v>
+      </c>
+      <c r="H8" t="n">
+        <v>47.42</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C9" t="n">
+        <v>63187</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5833</v>
+      </c>
+      <c r="E9" t="n">
+        <v>19505</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2341</v>
+      </c>
+      <c r="G9" t="n">
+        <v>30.87</v>
+      </c>
+      <c r="H9" t="n">
+        <v>40.13</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Montana</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C10" t="n">
+        <v>863</v>
+      </c>
+      <c r="D10" t="n">
+        <v>22</v>
+      </c>
+      <c r="E10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Alaska</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C11" t="n">
+        <v>883</v>
+      </c>
+      <c r="D11" t="n">
+        <v>14</v>
+      </c>
+      <c r="E11" t="n">
+        <v>23</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C12" t="n">
+        <v>108667</v>
+      </c>
+      <c r="D12" t="n">
+        <v>8060</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10162</v>
+      </c>
+      <c r="F12" t="n">
+        <v>665</v>
+      </c>
+      <c r="G12" t="n">
+        <v>9.35</v>
+      </c>
+      <c r="H12" t="n">
+        <v>8.25</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C13" t="n">
+        <v>20261</v>
+      </c>
+      <c r="D13" t="n">
+        <v>996</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3760</v>
+      </c>
+      <c r="F13" t="n">
+        <v>246</v>
+      </c>
+      <c r="G13" t="n">
+        <v>40.16</v>
+      </c>
+      <c r="H13" t="n">
+        <v>38.56</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>21100</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>167</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Mississippi</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C15" t="n">
+        <v>11766</v>
+      </c>
+      <c r="D15" t="n">
+        <v>506</v>
+      </c>
+      <c r="E15" t="n">
+        <v>27144</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1056</v>
+      </c>
+      <c r="G15" t="n">
+        <v>230.7</v>
+      </c>
+      <c r="H15" t="n">
+        <v>208.7</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Texas -- Bexar County</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C16" t="n">
+        <v>10147</v>
+      </c>
+      <c r="D16" t="n">
+        <v>109</v>
+      </c>
+      <c r="E16" t="n">
+        <v>430</v>
+      </c>
+      <c r="F16" t="n">
+        <v>17</v>
+      </c>
+      <c r="G16" t="n">
+        <v>7.32</v>
+      </c>
+      <c r="H16" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C17" t="n">
+        <v>35549</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1425</v>
+      </c>
+      <c r="E17" t="n">
+        <v>7457</v>
+      </c>
+      <c r="F17" t="n">
+        <v>115</v>
+      </c>
+      <c r="G17" t="n">
+        <v>20.98</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8.07</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Texas</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C18" t="n">
+        <v>21262</v>
+      </c>
+      <c r="D18" t="n">
+        <v>662</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2535</v>
+      </c>
+      <c r="F18" t="n">
+        <v>85</v>
+      </c>
+      <c r="G18" t="n">
+        <v>11.92</v>
+      </c>
+      <c r="H18" t="n">
+        <v>12.84</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Delaware</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C19" t="n">
+        <v>11226</v>
+      </c>
+      <c r="D19" t="n">
+        <v>507</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2970</v>
+      </c>
+      <c r="F19" t="n">
+        <v>130</v>
+      </c>
+      <c r="G19" t="n">
+        <v>26.46</v>
+      </c>
+      <c r="H19" t="n">
+        <v>25.64</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>142819</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>5711</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>6309</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>533</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>4.4</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>9.3</t>
+        </is>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Vermont</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>113</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>New Mexico</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C22" t="n">
+        <v>11809</v>
+      </c>
+      <c r="D22" t="n">
+        <v>492</v>
+      </c>
+      <c r="E22" t="n">
+        <v>227</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C23" t="n">
+        <v>138567</v>
+      </c>
+      <c r="D23" t="n">
+        <v>3419</v>
+      </c>
+      <c r="E23" t="n">
+        <v>20042</v>
+      </c>
+      <c r="F23" t="n">
+        <v>685</v>
+      </c>
+      <c r="G23" t="n">
+        <v>14.46</v>
+      </c>
+      <c r="H23" t="n">
+        <v>20.04</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Washington, DC</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C24" t="n">
+        <v>10248</v>
+      </c>
+      <c r="D24" t="n">
+        <v>550</v>
+      </c>
+      <c r="E24" t="n">
+        <v>5117</v>
+      </c>
+      <c r="F24" t="n">
+        <v>404</v>
+      </c>
+      <c r="G24" t="n">
+        <v>49.93</v>
+      </c>
+      <c r="H24" t="n">
+        <v>73.45</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C25" t="n">
+        <v>32307</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1676</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1747</v>
+      </c>
+      <c r="F25" t="n">
+        <v>108</v>
+      </c>
+      <c r="G25" t="n">
+        <v>5.41</v>
+      </c>
+      <c r="H25" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C26" t="n">
+        <v>13334</v>
+      </c>
+      <c r="D26" t="n">
+        <v>361</v>
+      </c>
+      <c r="E26" t="n">
+        <v>457</v>
+      </c>
+      <c r="F26" t="n">
+        <v>11</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4.24</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3.07</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C27" t="n">
+        <v>77210</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2778</v>
+      </c>
+      <c r="E27" t="n">
+        <v>22192</v>
+      </c>
+      <c r="F27" t="n">
+        <v>1319</v>
+      </c>
+      <c r="G27" t="n">
+        <v>28.74</v>
+      </c>
+      <c r="H27" t="n">
+        <v>47.48</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C28" t="n">
+        <v>61736</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1732</v>
+      </c>
+      <c r="E28" t="n">
+        <v>8771</v>
+      </c>
+      <c r="F28" t="n">
+        <v>379</v>
+      </c>
+      <c r="G28" t="n">
+        <v>14.21</v>
+      </c>
+      <c r="H28" t="n">
+        <v>21.88</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C29" t="n">
+        <v>44930</v>
+      </c>
+      <c r="D29" t="n">
+        <v>2427</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5513</v>
+      </c>
+      <c r="F29" t="n">
+        <v>355</v>
+      </c>
+      <c r="G29" t="n">
+        <v>12.27</v>
+      </c>
+      <c r="H29" t="n">
+        <v>14.63</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>44010</v>
+      </c>
+      <c r="C30" t="n">
+        <v>15232</v>
+      </c>
+      <c r="D30" t="n">
+        <v>558</v>
+      </c>
+      <c r="E30" t="n">
+        <v>1821</v>
+      </c>
+      <c r="F30" t="n">
+        <v>22</v>
+      </c>
+      <c r="G30" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="H30" t="n">
+        <v>4.19</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>California - Los Angeles</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C31" t="n">
+        <v>97894</v>
+      </c>
+      <c r="D31" t="n">
+        <v>3305</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2791</v>
+      </c>
+      <c r="F31" t="n">
+        <v>351</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2.85</v>
+      </c>
+      <c r="H31" t="n">
+        <v>10.62</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>